<commit_message>
DataImporter and data template update
</commit_message>
<xml_diff>
--- a/src/main/resources/EmployeeList.xlsx
+++ b/src/main/resources/EmployeeList.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cagrigurbuz\Desktop\dutyassignment\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD101A5E-76CF-4D81-AD20-2BD0104762AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8613473D-B361-4ABD-A2DD-A1B4FA4D1B69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="EmployeeList" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>